<commit_message>
note one to_predict files
</commit_message>
<xml_diff>
--- a/to_predict/UNverified_07292020.xlsx
+++ b/to_predict/UNverified_07292020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholamerkel/Library/Containers/com.microsoft.Excel/Data/Desktop/Work/NGC/sentiment analysis/covid/albert/to_predict/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholamerkel/Desktop/Work/NGC/sentiment analysis/covid/albert/to_predict/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BA81D9-C369-184F-ABC7-779C30DC5C5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E3D9F0-6AA2-3042-BE4B-20D718597988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="25480" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="983">
   <si>
     <t>text</t>
   </si>
@@ -2976,6 +2976,9 @@
   </si>
   <si>
     <t>x?</t>
+  </si>
+  <si>
+    <t>**predictions made with covid_output_unclean</t>
   </si>
 </sst>
 </file>
@@ -3344,7 +3347,7 @@
   <dimension ref="A1:G999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3450,6 +3453,9 @@
       <c r="C7">
         <v>1</v>
       </c>
+      <c r="E7" t="s">
+        <v>982</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">

</xml_diff>